<commit_message>
Added custom error pages
</commit_message>
<xml_diff>
--- a/storage/files/DTRTemplates/DTRSummaryReport.xlsx
+++ b/storage/files/DTRTemplates/DTRSummaryReport.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rienamae\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\hpo-hris\storage\files\DTRTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>